<commit_message>
most up to date python script
</commit_message>
<xml_diff>
--- a/SuperLiteData.xlsx
+++ b/SuperLiteData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbalusu/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbalusu/Desktop/SL/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15880" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -514,7 +514,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:J12"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -852,6 +852,9 @@
       <c r="J10" s="1">
         <v>34</v>
       </c>
+      <c r="L10" s="3">
+        <v>42976</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -884,6 +887,9 @@
       <c r="J11" s="1">
         <v>34</v>
       </c>
+      <c r="L11" s="3">
+        <v>42976</v>
+      </c>
       <c r="N11" t="s">
         <v>38</v>
       </c>
@@ -918,6 +924,9 @@
       </c>
       <c r="J12" s="1">
         <v>35.5</v>
+      </c>
+      <c r="L12" s="3">
+        <v>42978</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>